<commit_message>
Selecting the sheet in xlsx actually works now.
</commit_message>
<xml_diff>
--- a/samples/sample.xlsx
+++ b/samples/sample.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Base" sheetId="1" r:id="rId1"/>
+    <sheet name="Expansion" sheetId="2" r:id="rId2"/>
+    <sheet name="Resources" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -43,6 +43,27 @@
   </si>
   <si>
     <t>A clever pickpocket on the street.</t>
+  </si>
+  <si>
+    <t>Bootlegger</t>
+  </si>
+  <si>
+    <t>Rum Runner</t>
+  </si>
+  <si>
+    <t>Whiskey Baron</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -385,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -443,24 +464,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
xlsx,csv: trim whitespace, yield to optional block
Closes #108 and #79
</commit_message>
<xml_diff>
--- a/samples/sample.xlsx
+++ b/samples/sample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -54,23 +54,26 @@
     <t>Whiskey Baron</t>
   </si>
   <si>
-    <t>Wood</t>
-  </si>
-  <si>
-    <t>Metal</t>
-  </si>
-  <si>
-    <t>Stone</t>
-  </si>
-  <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wood                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metal                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stone                           </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +119,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -162,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,9 +205,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,6 +240,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,16 +416,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -434,7 +447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -445,7 +458,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -463,19 +476,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -491,7 +504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -499,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -513,43 +526,57 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>